<commit_message>
get_lunch_info_teacher, acception deleting class
</commit_message>
<xml_diff>
--- a/attendance_report.xlsx
+++ b/attendance_report.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="1" max="1"/>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -450,85 +450,58 @@
       <c r="A1" s="2" t="n"/>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>25.12.2024</t>
+          <t>09.01.2025</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>26.12.2024</t>
+          <t>10.01.2025</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>09.01.2025</t>
+          <t>13.01.2025</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>10.01.2025</t>
+          <t>12.01.2025</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Бородин Артём</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
+          <t>Точкееееееее Точкеее</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr"/>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>З</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
+      <c r="E2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Шекушев Филипп</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr"/>
+          <t>Шекшуев Филипп</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
       <c r="C3" s="2" t="inlineStr"/>
-      <c r="D3" s="2" t="inlineStr"/>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>З</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Шекшукв Филипп</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>З</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>З</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr"/>
+      <c r="E3" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
all users info in exel
</commit_message>
<xml_diff>
--- a/attendance_report.xlsx
+++ b/attendance_report.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,69 +439,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
     <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="n"/>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>09.01.2025</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>10.01.2025</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>13.01.2025</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>12.01.2025</t>
+          <t>20.01.2025</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Точкееееееее Точкеее</t>
+          <t>Точкее Точк</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr"/>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>З</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Шекшуев Филипп</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr"/>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>